<commit_message>
Primer Fix de la DB en SQL. Primer Stored Procedure, no funciona porque falta trabajo.
</commit_message>
<xml_diff>
--- a/DB y Operaciones de Usuario.xlsx
+++ b/DB y Operaciones de Usuario.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estudiantes Draft" sheetId="1" r:id="rId1"/>
     <sheet name="Diagrama Completo" sheetId="3" r:id="rId2"/>
-    <sheet name="Operaciones de Usuario" sheetId="4" r:id="rId3"/>
+    <sheet name="Diagrama Completo (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="Operaciones de Usuario" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="233">
   <si>
     <t>Teléfonos</t>
   </si>
@@ -758,11 +759,53 @@
   <si>
     <t xml:space="preserve">Preferí dejarte a vos eso ya que sabes exactamente a que se debe lo que hiciste y puede que yo haya entendido mal algo. </t>
   </si>
+  <si>
+    <t>https://stackoverflow.com/questions/5835978/how-to-properly-create-composite-primary-keys-mysql</t>
+  </si>
+  <si>
+    <t>Gris</t>
+  </si>
+  <si>
+    <t>Resuelto por Diego</t>
+  </si>
+  <si>
+    <t>id_asignacion_estudiante: int(11)</t>
+  </si>
+  <si>
+    <t>id_asignacion_catedratico: int(11)</t>
+  </si>
+  <si>
+    <t>Ya le puse una llave primaria doble, que usa esas dos foráneas.</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>*id_asignacion_catedratico: int(11)</t>
+  </si>
+  <si>
+    <t>Los tres campos en color piel son llaves primarias, y id_asignacion_catedratico es foranea a la vez. Gracias por el cambio del nombre de esa.</t>
+  </si>
+  <si>
+    <t>PendienteS:</t>
+  </si>
+  <si>
+    <t>Corregir empleado_trabajando a empleadoS_trabajando porque está mal especificado</t>
+  </si>
+  <si>
+    <t>El campo expedienteen_VCR se llama expedienteS_VCR. Corregir.</t>
+  </si>
+  <si>
+    <t>Especificar este constraint en empleados_laborando</t>
+  </si>
+  <si>
+    <t>Especificar este constraint en roles_de_sistema</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,7 +838,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,6 +884,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1316,6 +1371,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1352,22 +1421,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3338,6 +3409,1979 @@
         <a:xfrm flipH="1">
           <a:off x="14345228" y="6999432"/>
           <a:ext cx="2597727" cy="3449204"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19052</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector recto 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8001002" y="2912165"/>
+          <a:ext cx="1835424" cy="535885"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>9719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19245</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13792201" y="10125269"/>
+          <a:ext cx="0" cy="390526"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>321624</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5248275" y="4476750"/>
+          <a:ext cx="1093149" cy="600076"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1025769</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>831272</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>17320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2168769" y="9734550"/>
+          <a:ext cx="10054403" cy="17320"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>757331</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5253131" y="3887134"/>
+          <a:ext cx="798419" cy="14941"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>940130</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>160812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>942976</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6959930" y="4447062"/>
+          <a:ext cx="2846" cy="620238"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7989277" y="4476750"/>
+          <a:ext cx="745148" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>182218</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2190750" y="5979102"/>
+          <a:ext cx="1406200" cy="261016"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>17319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Conector recto 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2190750" y="5275119"/>
+          <a:ext cx="1400175" cy="105145"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15127</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15127</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4510927" y="6450106"/>
+          <a:ext cx="0" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector recto 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7991475" y="5867401"/>
+          <a:ext cx="342900" cy="752474"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352428</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>3</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector recto 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7791450" y="4491404"/>
+          <a:ext cx="542928" cy="1366474"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector recto 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4486275" y="8553450"/>
+          <a:ext cx="9525" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>327421</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Conector recto 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4495800" y="8848725"/>
+          <a:ext cx="7223521" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>329045</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>335056</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>98502</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11720945" y="7583632"/>
+          <a:ext cx="6011" cy="1277870"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>732694</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7952644" y="3996105"/>
+          <a:ext cx="4296506" cy="35772"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>70758</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>20864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector recto 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9824358" y="2895600"/>
+          <a:ext cx="4996542" cy="20864"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>489859</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14834509" y="1189264"/>
+          <a:ext cx="13605" cy="1731184"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>88079</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>92592</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>46452</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12337229" y="2498124"/>
+          <a:ext cx="4513" cy="443928"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>410070</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>421821</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>31210</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector recto 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10935195" y="1393371"/>
+          <a:ext cx="11751" cy="1533439"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>10948</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>175173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15461</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47788</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector recto 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10536073" y="2289723"/>
+          <a:ext cx="4513" cy="653665"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1073515</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>187377</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>7808</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector recto 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="20437840" y="2301927"/>
+          <a:ext cx="905968" cy="3123"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>750794</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>753009</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27715</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector recto 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7970744" y="6037169"/>
+          <a:ext cx="764215" cy="619946"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1021773</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1039091</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector recto 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2164773" y="7393132"/>
+          <a:ext cx="17318" cy="2358736"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1039093</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>17319</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector recto 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2182093" y="6438900"/>
+          <a:ext cx="1408832" cy="988869"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector recto 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14344650" y="10687050"/>
+          <a:ext cx="1114425" cy="396875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581396</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>583321</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector recto 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13887821" y="2895600"/>
+          <a:ext cx="1925" cy="782782"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>434883</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>17320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector recto 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="14367062" y="2886075"/>
+          <a:ext cx="2346046" cy="826945"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>606137</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>623455</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector recto 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18113087" y="954232"/>
+          <a:ext cx="17318" cy="2741468"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>624758</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector recto 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="18131708" y="971550"/>
+          <a:ext cx="642067" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Conector recto 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="18792825" y="4286250"/>
+          <a:ext cx="819151" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector recto 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="18792825" y="5067300"/>
+          <a:ext cx="819151" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector recto 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="21355050" y="4286250"/>
+          <a:ext cx="1066801" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Conector recto 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="21364575" y="5267325"/>
+          <a:ext cx="1057277" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="22433056" y="3274920"/>
+          <a:ext cx="0" cy="420781"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>2081</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Conector recto 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12249150" y="3274919"/>
+          <a:ext cx="10174781" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134472</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector recto 37"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12249151" y="3263714"/>
+          <a:ext cx="11205" cy="756958"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>389659</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>616877</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Conector recto 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11781559" y="7600950"/>
+          <a:ext cx="10171318" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>536864</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>554183</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Conector recto 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="21872864" y="3661064"/>
+          <a:ext cx="17319" cy="3957204"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>526677</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Conector recto 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="21358411" y="3706906"/>
+          <a:ext cx="504266" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9506</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>24423</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Conector recto 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="17506950" y="5857877"/>
+          <a:ext cx="4924406" cy="4091596"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>17322</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>10281</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Conector recto 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="23372622" y="6638925"/>
+          <a:ext cx="1728" cy="1553331"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Conector recto 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13765866" y="5876925"/>
+          <a:ext cx="2531409" cy="3299011"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>620569</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Conector recto 44"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14344651" y="7019925"/>
+          <a:ext cx="2554143" cy="3476625"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3829,10 +5873,10 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="106"/>
+      <c r="C14" s="118"/>
       <c r="F14" s="3"/>
       <c r="H14" s="1" t="s">
         <v>48</v>
@@ -3911,8 +5955,8 @@
         <v>6</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
       <c r="K20" s="12" t="s">
         <v>46</v>
       </c>
@@ -3927,10 +5971,10 @@
       <c r="E21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="105" t="s">
+      <c r="K21" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="105"/>
+      <c r="L21" s="117"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -3961,10 +6005,10 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="106" t="s">
+      <c r="B24" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="106"/>
+      <c r="C24" s="118"/>
       <c r="E24" t="s">
         <v>55</v>
       </c>
@@ -4017,10 +6061,10 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="107" t="s">
+      <c r="H30" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="107"/>
+      <c r="I30" s="119"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
@@ -4045,10 +6089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB76"/>
+  <dimension ref="A1:AB79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z46" sqref="Z46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4098,16 +6142,16 @@
       <c r="J3" s="70"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-      <c r="M3" s="123" t="s">
+      <c r="M3" s="112" t="s">
         <v>101</v>
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
-      <c r="Q3" s="119" t="s">
+      <c r="Q3" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="121"/>
+      <c r="R3" s="110"/>
       <c r="S3" s="71"/>
       <c r="U3" s="67"/>
       <c r="V3" s="68"/>
@@ -4135,7 +6179,7 @@
       <c r="R4" s="17"/>
       <c r="S4" s="56"/>
       <c r="U4" s="70"/>
-      <c r="V4" s="119" t="s">
+      <c r="V4" s="108" t="s">
         <v>138</v>
       </c>
       <c r="W4" s="15"/>
@@ -4212,10 +6256,10 @@
       <c r="R7" s="12"/>
       <c r="S7" s="71"/>
       <c r="U7" s="70"/>
-      <c r="V7" s="108" t="s">
+      <c r="V7" s="120" t="s">
         <v>141</v>
       </c>
-      <c r="W7" s="109"/>
+      <c r="W7" s="121"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="14" t="s">
         <v>129</v>
@@ -4252,7 +6296,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
-      <c r="O9" s="123" t="s">
+      <c r="O9" s="112" t="s">
         <v>2</v>
       </c>
       <c r="P9" s="15"/>
@@ -4273,10 +6317,10 @@
     </row>
     <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="J10" s="70"/>
-      <c r="K10" s="119" t="s">
+      <c r="K10" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="121"/>
+      <c r="L10" s="110"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="16" t="s">
@@ -4458,12 +6502,12 @@
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="118" t="s">
+      <c r="E18" s="107" t="s">
         <v>48</v>
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="72"/>
-      <c r="H18" s="119" t="s">
+      <c r="H18" s="108" t="s">
         <v>1</v>
       </c>
       <c r="I18" s="15"/>
@@ -4551,26 +6595,26 @@
       <c r="L20" s="12"/>
       <c r="M20" s="71"/>
       <c r="O20" s="70"/>
-      <c r="P20" s="119" t="s">
+      <c r="P20" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="Q20" s="121"/>
+      <c r="Q20" s="110"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
-      <c r="T20" s="119" t="s">
+      <c r="T20" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="U20" s="121"/>
+      <c r="U20" s="110"/>
       <c r="V20" s="12"/>
-      <c r="W20" s="119" t="s">
+      <c r="W20" s="108" t="s">
         <v>93</v>
       </c>
       <c r="X20" s="15"/>
       <c r="Y20" s="12"/>
-      <c r="Z20" s="119" t="s">
+      <c r="Z20" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="AA20" s="121"/>
+      <c r="AA20" s="110"/>
       <c r="AB20" s="71"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4747,7 +6791,7 @@
       <c r="AB24" s="71"/>
     </row>
     <row r="25" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="106" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="43"/>
@@ -4772,7 +6816,7 @@
       </c>
       <c r="U25" s="19"/>
       <c r="V25" s="12"/>
-      <c r="W25" s="119" t="s">
+      <c r="W25" s="108" t="s">
         <v>104</v>
       </c>
       <c r="X25" s="15"/>
@@ -4833,17 +6877,17 @@
       <c r="D27" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="121"/>
+      <c r="F27" s="110"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="119" t="s">
+      <c r="H27" s="108" t="s">
         <v>100</v>
       </c>
       <c r="I27" s="15"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="119" t="s">
+      <c r="K27" s="108" t="s">
         <v>16</v>
       </c>
       <c r="L27" s="15"/>
@@ -4869,10 +6913,10 @@
       <c r="Y27" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="Z27" s="119" t="s">
+      <c r="Z27" s="108" t="s">
         <v>105</v>
       </c>
-      <c r="AA27" s="121"/>
+      <c r="AA27" s="110"/>
       <c r="AB27" s="71"/>
     </row>
     <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4883,7 +6927,7 @@
       <c r="C28" s="13"/>
       <c r="D28" s="12"/>
       <c r="E28" s="24" t="s">
-        <v>25</v>
+        <v>222</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="12"/>
@@ -4913,7 +6957,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="Z28" s="61" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="AA28" s="17"/>
       <c r="AB28" s="71"/>
@@ -5007,7 +7051,7 @@
       <c r="AB30" s="71"/>
     </row>
     <row r="31" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="117" t="s">
+      <c r="A31" s="106" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="43"/>
@@ -5068,10 +7112,10 @@
         <v>71</v>
       </c>
       <c r="J32" s="12"/>
-      <c r="K32" s="115" t="s">
+      <c r="K32" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="L32" s="116"/>
+      <c r="L32" s="128"/>
       <c r="M32" s="71"/>
       <c r="O32" s="70"/>
       <c r="P32" s="12"/>
@@ -5180,14 +7224,14 @@
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="119" t="s">
+      <c r="H35" s="108" t="s">
         <v>63</v>
       </c>
       <c r="I35" s="36"/>
       <c r="J35" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K35" s="119" t="s">
+      <c r="K35" s="108" t="s">
         <v>135</v>
       </c>
       <c r="L35" s="15"/>
@@ -5255,7 +7299,7 @@
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="E37" s="120" t="s">
+      <c r="E37" s="109" t="s">
         <v>60</v>
       </c>
       <c r="F37" s="15"/>
@@ -5302,10 +7346,10 @@
       </c>
       <c r="I38" s="35"/>
       <c r="J38" s="12"/>
-      <c r="K38" s="115" t="s">
+      <c r="K38" s="127" t="s">
         <v>35</v>
       </c>
-      <c r="L38" s="116"/>
+      <c r="L38" s="128"/>
       <c r="M38" s="71"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
@@ -5368,8 +7412,8 @@
       </c>
       <c r="I40" s="40"/>
       <c r="J40" s="12"/>
-      <c r="K40" s="114"/>
-      <c r="L40" s="114"/>
+      <c r="K40" s="126"/>
+      <c r="L40" s="126"/>
       <c r="M40" s="71"/>
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
@@ -5423,25 +7467,25 @@
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
-      <c r="E43" s="112" t="s">
+      <c r="E43" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="113"/>
+      <c r="F43" s="125"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="110" t="s">
+      <c r="H43" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="I43" s="111"/>
+      <c r="I43" s="123"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="71"/>
       <c r="Y43" s="55"/>
-      <c r="Z43" s="119" t="s">
+      <c r="Z43" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="AA43" s="121"/>
-      <c r="AB43" s="56"/>
+      <c r="AA43" s="110"/>
+      <c r="AB43" s="130"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="70"/>
@@ -5461,7 +7505,7 @@
       <c r="M44" s="71"/>
       <c r="Y44" s="55"/>
       <c r="Z44" s="61" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="AA44" s="21"/>
       <c r="AB44" s="56"/>
@@ -5519,7 +7563,7 @@
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N48" s="70"/>
-      <c r="O48" s="120" t="s">
+      <c r="O48" s="109" t="s">
         <v>8</v>
       </c>
       <c r="P48" s="29"/>
@@ -5596,7 +7640,7 @@
       </c>
       <c r="P52" s="23"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="122" t="s">
+      <c r="R52" s="111" t="s">
         <v>113</v>
       </c>
       <c r="S52" s="92"/>
@@ -5605,6 +7649,7 @@
       <c r="V52" s="12"/>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
       <c r="N53" s="70"/>
       <c r="O53" s="12"/>
       <c r="P53" s="12" t="s">
@@ -5637,7 +7682,7 @@
         <v>191</v>
       </c>
       <c r="N55" s="70"/>
-      <c r="O55" s="120" t="s">
+      <c r="O55" s="109" t="s">
         <v>12</v>
       </c>
       <c r="P55" s="29"/>
@@ -5652,7 +7697,7 @@
       <c r="U55" s="71"/>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A56" s="124" t="s">
+      <c r="A56" s="113" t="s">
         <v>192</v>
       </c>
       <c r="B56" t="s">
@@ -5672,7 +7717,7 @@
       <c r="U56" s="71"/>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A57" s="125" t="s">
+      <c r="A57" s="114" t="s">
         <v>194</v>
       </c>
       <c r="B57" t="s">
@@ -5690,10 +7735,10 @@
       <c r="U57" s="71"/>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A58" s="124" t="s">
+      <c r="A58" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="B58" s="125" t="s">
+      <c r="B58" s="114" t="s">
         <v>194</v>
       </c>
       <c r="C58" t="s">
@@ -5716,7 +7761,7 @@
       <c r="U58" s="71"/>
     </row>
     <row r="59" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="126" t="s">
+      <c r="A59" s="115" t="s">
         <v>197</v>
       </c>
       <c r="B59" t="s">
@@ -5731,8 +7776,16 @@
       <c r="T59" s="74"/>
       <c r="U59" s="75"/>
     </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A60" s="129" t="s">
+        <v>220</v>
+      </c>
+      <c r="B60" t="s">
+        <v>221</v>
+      </c>
+    </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A62" s="127" t="s">
+      <c r="A62" s="116" t="s">
         <v>199</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -5755,7 +7808,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -5766,7 +7819,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -5777,7 +7830,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>27</v>
       </c>
@@ -5785,7 +7838,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -5793,7 +7846,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -5801,31 +7854,53 @@
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="129" t="s">
         <v>210</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="129" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="C70" s="129"/>
+      <c r="F70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="129" t="s">
         <v>212</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="129" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="H71" s="129"/>
+      <c r="I71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="129" t="s">
         <v>213</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="129" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="129"/>
+      <c r="D72" s="129"/>
+      <c r="E72" s="129"/>
+      <c r="F72" s="129"/>
+      <c r="G72" s="129"/>
+      <c r="H72" s="129"/>
+      <c r="I72" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>214</v>
       </c>
@@ -5833,9 +7908,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -5848,7 +7928,7 @@
     <mergeCell ref="K32:L32"/>
   </mergeCells>
   <conditionalFormatting sqref="E33 J27 J33:K33 E27:F30 K34">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5858,10 +7938,1933 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="19" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1"/>
+    <col min="26" max="26" width="14" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="69"/>
+    </row>
+    <row r="3" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J3" s="70"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="108" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="110"/>
+      <c r="S3" s="71"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y3" s="68"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="69"/>
+    </row>
+    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J4" s="70"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="56"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="W4" s="110"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="71"/>
+    </row>
+    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J5" s="70"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="19"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="19"/>
+      <c r="S5" s="56"/>
+      <c r="U5" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="W5" s="17"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="71"/>
+    </row>
+    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J6" s="70"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="19"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="23"/>
+      <c r="S6" s="56"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="W6" s="19"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="71"/>
+    </row>
+    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J7" s="70"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="12"/>
+      <c r="S7" s="71"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="W7" s="121"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="71"/>
+    </row>
+    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J8" s="70"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="71"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="71"/>
+    </row>
+    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J9" s="70"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="112" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="71"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="W9" s="15"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="71"/>
+    </row>
+    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J10" s="70"/>
+      <c r="K10" s="108" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="110"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="71"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="W10" s="17"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="71"/>
+    </row>
+    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J11" s="70"/>
+      <c r="K11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="71"/>
+      <c r="U11" s="70"/>
+      <c r="V11" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="W11" s="19"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="71"/>
+    </row>
+    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J12" s="70"/>
+      <c r="K12" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="28"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="71"/>
+      <c r="U12" s="70"/>
+      <c r="V12" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="W12" s="19"/>
+      <c r="X12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y12" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z12" s="65"/>
+      <c r="AA12" s="71"/>
+    </row>
+    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="J13" s="70"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="71"/>
+      <c r="U13" s="70"/>
+      <c r="V13" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="W13" s="19"/>
+      <c r="X13" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y13" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="71"/>
+    </row>
+    <row r="14" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="13"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="75"/>
+      <c r="U14" s="70"/>
+      <c r="V14" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="W14" s="23"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="71"/>
+    </row>
+    <row r="15" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="13"/>
+      <c r="N15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="U15" s="73"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="74"/>
+      <c r="X15" s="74"/>
+      <c r="Y15" s="74"/>
+      <c r="Z15" s="74"/>
+      <c r="AA15" s="75"/>
+    </row>
+    <row r="16" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="67"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="69"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+    </row>
+    <row r="18" spans="1:28" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="49"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="71"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="50"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="71"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="85" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q19" s="68"/>
+      <c r="R19" s="68"/>
+      <c r="S19" s="68"/>
+      <c r="T19" s="84" t="s">
+        <v>70</v>
+      </c>
+      <c r="U19" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="V19" s="68"/>
+      <c r="W19" s="68"/>
+      <c r="X19" s="68"/>
+      <c r="Y19" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z19" s="68"/>
+      <c r="AA19" s="68"/>
+      <c r="AB19" s="69"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="70"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="71"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="U20" s="110"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="108" t="s">
+        <v>93</v>
+      </c>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA20" s="131"/>
+      <c r="AB20" s="71"/>
+    </row>
+    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="70"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="48"/>
+      <c r="G21" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="71"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="U21" s="17"/>
+      <c r="V21" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="W21" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="71"/>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="70"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="19"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="71"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="U22" s="19"/>
+      <c r="V22" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="W22" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z22" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="71"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="70"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="71"/>
+      <c r="O23" s="70"/>
+      <c r="P23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="U23" s="19"/>
+      <c r="V23" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="W23" s="95" t="s">
+        <v>96</v>
+      </c>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="71"/>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="70"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="71"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="U24" s="19"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="71"/>
+    </row>
+    <row r="25" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="106" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="71"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="U25" s="19"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="108" t="s">
+        <v>104</v>
+      </c>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="12"/>
+      <c r="AB25" s="71"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="45"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="71"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="U26" s="19"/>
+      <c r="V26" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="W26" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB26" s="71"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="46"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="108" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="110"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="108" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27" s="15"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" s="15"/>
+      <c r="M27" s="71"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="U27" s="19"/>
+      <c r="V27" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="W27" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z27" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA27" s="131"/>
+      <c r="AB27" s="71"/>
+    </row>
+    <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="48"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="71"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="U28" s="19"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="61" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="71"/>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="70"/>
+      <c r="B29" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="63"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="71"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="U29" s="19"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA29" s="21"/>
+      <c r="AB29" s="71"/>
+    </row>
+    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="70"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="I30" s="66"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L30" s="19"/>
+      <c r="M30" s="71"/>
+      <c r="O30" s="70"/>
+      <c r="P30" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="T30" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="U30" s="19"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z30" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA30" s="21"/>
+      <c r="AB30" s="71"/>
+    </row>
+    <row r="31" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="106" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="43"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="21"/>
+      <c r="M31" s="71"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="U31" s="19"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA31" s="63"/>
+      <c r="AB31" s="71"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" s="88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="45"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" s="12"/>
+      <c r="K32" s="127" t="s">
+        <v>38</v>
+      </c>
+      <c r="L32" s="128"/>
+      <c r="M32" s="71"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="U32" s="19"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="71"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A33" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="105" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="71"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="U33" s="19"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="71"/>
+    </row>
+    <row r="34" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="48"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L34" s="12"/>
+      <c r="M34" s="71"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="U34" s="19"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA34" s="65"/>
+      <c r="AB34" s="71"/>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="90"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="108" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" s="36"/>
+      <c r="J35" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="L35" s="15"/>
+      <c r="M35" s="71"/>
+      <c r="O35" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="U35" s="19"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB35" s="71"/>
+    </row>
+    <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="70"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="37"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="L36" s="17"/>
+      <c r="M36" s="71"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="U36" s="23"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="71"/>
+    </row>
+    <row r="37" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="70"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" s="35"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="L37" s="19"/>
+      <c r="M37" s="71"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="74"/>
+      <c r="S37" s="74"/>
+      <c r="T37" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
+      <c r="X37" s="74"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="74"/>
+      <c r="AA37" s="74"/>
+      <c r="AB37" s="75"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A38" s="70"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="35"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="127" t="s">
+        <v>35</v>
+      </c>
+      <c r="L38" s="128"/>
+      <c r="M38" s="71"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+      <c r="W38" s="12"/>
+      <c r="X38" s="12"/>
+      <c r="Y38" s="12"/>
+      <c r="Z38" s="12"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="12"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A39" s="70"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="21"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39" s="35"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="71"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="12"/>
+      <c r="Z39" s="12"/>
+      <c r="AA39" s="12"/>
+      <c r="AB39" s="12"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A40" s="70"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="33"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="40"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="126"/>
+      <c r="L40" s="126"/>
+      <c r="M40" s="71"/>
+      <c r="Y40" s="12"/>
+      <c r="Z40" s="12"/>
+    </row>
+    <row r="41" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="70"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="35"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="71"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A42" s="70"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="19"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="33"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="71"/>
+      <c r="Y42" s="52"/>
+      <c r="Z42" s="53"/>
+      <c r="AA42" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB42" s="54"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A43" s="70"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="124" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="125"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="122" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" s="123"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="71"/>
+      <c r="Y43" s="55"/>
+      <c r="Z43" s="108" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA43" s="131"/>
+      <c r="AB43" s="56"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A44" s="70"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="26"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="71"/>
+      <c r="Y44" s="55"/>
+      <c r="Z44" s="61" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA44" s="21"/>
+      <c r="AB44" s="56"/>
+    </row>
+    <row r="45" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="73"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
+      <c r="M45" s="75"/>
+      <c r="Y45" s="55"/>
+      <c r="Z45" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA45" s="17"/>
+      <c r="AB45" s="56"/>
+    </row>
+    <row r="46" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X46" s="12"/>
+      <c r="Y46" s="55"/>
+      <c r="Z46" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA46" s="17"/>
+      <c r="AB46" s="56"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N47" s="67"/>
+      <c r="O47" s="68"/>
+      <c r="P47" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="68"/>
+      <c r="S47" s="68"/>
+      <c r="T47" s="68"/>
+      <c r="U47" s="69"/>
+      <c r="X47" s="12"/>
+      <c r="Y47" s="55"/>
+      <c r="Z47" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA47" s="63"/>
+      <c r="AB47" s="56"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N48" s="70"/>
+      <c r="O48" s="109" t="s">
+        <v>8</v>
+      </c>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="S48" s="60"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="71"/>
+      <c r="Y48" s="55"/>
+      <c r="Z48" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA48" s="63"/>
+      <c r="AB48" s="56"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N49" s="70"/>
+      <c r="O49" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P49" s="30"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="71"/>
+      <c r="Y49" s="55"/>
+      <c r="Z49" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA49" s="65"/>
+      <c r="AB49" s="56"/>
+    </row>
+    <row r="50" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N50" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="O50" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="71"/>
+      <c r="Y50" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z50" s="58"/>
+      <c r="AA50" s="58"/>
+      <c r="AB50" s="59"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N51" s="70"/>
+      <c r="O51" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="U51" s="71"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N52" s="70"/>
+      <c r="O52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="111" t="s">
+        <v>113</v>
+      </c>
+      <c r="S52" s="92"/>
+      <c r="T52" s="77"/>
+      <c r="U52" s="71"/>
+      <c r="V52" s="12"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="N53" s="70"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="S53" s="34"/>
+      <c r="T53" s="79"/>
+      <c r="U53" s="71"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N54" s="70"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="S54" s="12"/>
+      <c r="T54" s="81"/>
+      <c r="U54" s="71"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="N55" s="70"/>
+      <c r="O55" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="R55" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="S55" s="93"/>
+      <c r="T55" s="83"/>
+      <c r="U55" s="71"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A56" s="113" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" t="s">
+        <v>193</v>
+      </c>
+      <c r="N56" s="70"/>
+      <c r="O56" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="S56" s="87"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="71"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A57" s="114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" t="s">
+        <v>195</v>
+      </c>
+      <c r="N57" s="70"/>
+      <c r="O57" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="71"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A58" s="113" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="114" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" t="s">
+        <v>196</v>
+      </c>
+      <c r="G58" t="s">
+        <v>206</v>
+      </c>
+      <c r="N58" s="70"/>
+      <c r="O58" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="71"/>
+    </row>
+    <row r="59" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="115" t="s">
+        <v>197</v>
+      </c>
+      <c r="B59" t="s">
+        <v>198</v>
+      </c>
+      <c r="N59" s="73"/>
+      <c r="O59" s="74"/>
+      <c r="P59" s="74"/>
+      <c r="Q59" s="74"/>
+      <c r="R59" s="74"/>
+      <c r="S59" s="74"/>
+      <c r="T59" s="74"/>
+      <c r="U59" s="75"/>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A60" s="129" t="s">
+        <v>220</v>
+      </c>
+      <c r="B60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A62" s="116" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H65" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>204</v>
+      </c>
+      <c r="H66" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="129" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="129" t="s">
+        <v>211</v>
+      </c>
+      <c r="C70" s="129"/>
+      <c r="F70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="129" t="s">
+        <v>212</v>
+      </c>
+      <c r="B71" s="129" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="H71" s="129"/>
+      <c r="I71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="129" t="s">
+        <v>213</v>
+      </c>
+      <c r="B72" s="129" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" s="129"/>
+      <c r="D72" s="129"/>
+      <c r="E72" s="129"/>
+      <c r="F72" s="129"/>
+      <c r="G72" s="129"/>
+      <c r="H72" s="129"/>
+      <c r="I72" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="129" t="s">
+        <v>214</v>
+      </c>
+      <c r="B73" s="129" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="129"/>
+      <c r="D73" s="129"/>
+      <c r="E73" s="129"/>
+      <c r="F73" s="129"/>
+      <c r="G73" s="129"/>
+      <c r="H73" s="129"/>
+      <c r="I73" s="129"/>
+      <c r="J73" s="129"/>
+      <c r="K73" s="129"/>
+      <c r="L73" s="129"/>
+      <c r="M73" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" s="19"/>
+      <c r="C85" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="19"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" s="19"/>
+      <c r="C87" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="19"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="19"/>
+      <c r="C89" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="B90" s="121"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="H43:I43"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E33 J27 J33:K33 E27:F30 K34">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>